<commit_message>
Support for Dataset B
</commit_message>
<xml_diff>
--- a/Spreadsheets/Analytics.xlsx
+++ b/Spreadsheets/Analytics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samcoburn/Documents/School Files/Columbia Files/Spring 2022/COMS 6156/COMS6156_FinalProject/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0FC9E6-9CDC-2847-97A8-6862D3A5534F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DC41EC-D030-3D45-9832-445305B1F188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="500" windowWidth="18100" windowHeight="15880" xr2:uid="{FFE897EF-CC1A-114C-953C-A7E1FE5B8A2E}"/>
+    <workbookView xWindow="8940" yWindow="500" windowWidth="19860" windowHeight="15820" xr2:uid="{FFE897EF-CC1A-114C-953C-A7E1FE5B8A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Tool</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>TN</t>
+  </si>
+  <si>
+    <t>Java-Large</t>
+  </si>
+  <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
   </si>
 </sst>
 </file>
@@ -443,57 +452,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E865E5F3-CE15-C140-8EC1-D46FE3EB7CC3}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -504,119 +512,268 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>66</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>452</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>8780</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>220</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>548</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.4103</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.67259999999999998</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.45200000000000001</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.8125</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.54069999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>86</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>658</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>9000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>342</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.42920000000000003</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.65800000000000003</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.8891</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.79369999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>76</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>734</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8972</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>28</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>266</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.43140000000000001</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.96330000000000005</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.73399999999999999</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.92100000000000004</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.83309999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>87</v>
+      </c>
+      <c r="E7">
+        <v>344</v>
+      </c>
+      <c r="F7">
+        <v>8988</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>656</v>
+      </c>
+      <c r="I7">
+        <v>0.4148</v>
+      </c>
+      <c r="J7">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="K7">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="L7">
+        <v>0.83009999999999995</v>
+      </c>
+      <c r="M7">
+        <v>0.50739999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>91</v>
+      </c>
+      <c r="E8">
+        <v>628</v>
+      </c>
+      <c r="F8">
+        <v>9000</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>372</v>
+      </c>
+      <c r="I8">
+        <v>0.4279</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.628</v>
+      </c>
+      <c r="L8">
+        <v>0.87380000000000002</v>
+      </c>
+      <c r="M8">
+        <v>0.77149999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>88</v>
+      </c>
+      <c r="E9">
+        <v>788</v>
+      </c>
+      <c r="F9">
+        <v>8976</v>
+      </c>
+      <c r="G9">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>212</v>
+      </c>
+      <c r="I9">
+        <v>0.43390000000000001</v>
+      </c>
+      <c r="J9">
+        <v>0.97040000000000004</v>
+      </c>
+      <c r="K9">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="L9">
+        <v>0.92079999999999995</v>
+      </c>
+      <c r="M9">
+        <v>0.86980000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Upload of codeembeddings.py
</commit_message>
<xml_diff>
--- a/Spreadsheets/Analytics.xlsx
+++ b/Spreadsheets/Analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samcoburn/Documents/School Files/Columbia Files/Spring 2022/COMS 6156/COMS6156_FinalProject/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B882C6D-15BF-EC45-8A14-EE7C4B8EEC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D916237-B4A4-F847-866B-EB4B2D0E80D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="2" xr2:uid="{FFE897EF-CC1A-114C-953C-A7E1FE5B8A2E}"/>
   </bookViews>
@@ -990,13 +990,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEBEF3A-9650-0E43-9F43-0C39B0DBBFA3}">
   <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>

</xml_diff>